<commit_message>
Funciones de manejo de excel
</commit_message>
<xml_diff>
--- a/TABLA MATERIALES TP1.xlsx
+++ b/TABLA MATERIALES TP1.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quim\Dropbox\Acoustics Psychoacoustics Students\Mod II\Trabajos Prácticos\AYUDA TP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba58f79a5dcad87f/Escritorio/facultad/materias/Acústica y Psicoacústica II/AyP2-mod2-TP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_40917692348679852D654D4121B13106FDDC88C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD0909B0-A4EE-4DD7-95E7-60C9C8E31451}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Material</t>
   </si>
@@ -84,12 +96,15 @@
   </si>
   <si>
     <t>Densidad</t>
+  </si>
+  <si>
+    <t>Prueba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00E+000"/>
   </numFmts>
@@ -462,24 +477,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
@@ -499,7 +514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -519,7 +534,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -539,7 +554,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -559,7 +574,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -579,7 +594,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -599,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -619,7 +634,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -639,7 +654,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -659,7 +674,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -680,7 +695,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -700,7 +715,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -720,7 +735,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -740,7 +755,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -760,7 +775,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -778,6 +793,26 @@
       </c>
       <c r="G16" s="2">
         <v>0.24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>2888</v>
+      </c>
+      <c r="E17">
+        <v>200000000000</v>
+      </c>
+      <c r="F17">
+        <v>1E-4</v>
+      </c>
+      <c r="G17">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GUI - Lista de materiales
</commit_message>
<xml_diff>
--- a/TABLA MATERIALES TP1.xlsx
+++ b/TABLA MATERIALES TP1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba58f79a5dcad87f/Escritorio/facultad/materias/Acústica y Psicoacústica II/AyP2-mod2-TP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_40917692348679852D654D4121B13106FDDC88C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD0909B0-A4EE-4DD7-95E7-60C9C8E31451}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_40917692348679852D654D4121B13106FDDC88C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A753B696-10D6-4EF6-8505-52DCACFE0B5B}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Material</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Densidad</t>
-  </si>
-  <si>
-    <t>Prueba</t>
   </si>
 </sst>
 </file>
@@ -213,6 +210,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G17"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,26 +796,6 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17">
-        <v>2888</v>
-      </c>
-      <c r="E17">
-        <v>200000000000</v>
-      </c>
-      <c r="F17">
-        <v>1E-4</v>
-      </c>
-      <c r="G17">
-        <v>0.12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregar material - Funcionalidad terminada
</commit_message>
<xml_diff>
--- a/TABLA MATERIALES TP1.xlsx
+++ b/TABLA MATERIALES TP1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba58f79a5dcad87f/Escritorio/facultad/materias/Acústica y Psicoacústica II/AyP2-mod2-TP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_40917692348679852D654D4121B13106FDDC88C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A753B696-10D6-4EF6-8505-52DCACFE0B5B}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_40917692348679852D654D4121B13106FDDC88C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28950D82-FF6B-4585-9852-441EB1890C68}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,6 +195,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,10 +211,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,6 +793,9 @@
         <v>0.24</v>
       </c>
     </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E17" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>